<commit_message>
app/core to add diagrams to project and iac/data for project
</commit_message>
<xml_diff>
--- a/iac/data/xlsx/project.xlsx
+++ b/iac/data/xlsx/project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\WebstormProjects\Resume\iac\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCAE14E-D9AA-45D0-929B-B21F372CFEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1489295E-74C1-4BC5-92C2-8BE540D8D32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>description</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create a serverless Resume website hosted on three cloud providers. I chose to use AWS, Azure, and GCP. The frontend code is written in Angular. The backend code is written in Java. Infrastructure is managed by Terraform. CI/CD is managed by GitHub Actions. DNS is managed by AWS Route 53. </t>
+  </si>
+  <si>
+    <t>diagrams</t>
   </si>
 </sst>
 </file>
@@ -1209,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1222,16 +1225,17 @@
     <col min="3" max="3" width="74.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="6" width="11.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -1247,26 +1251,29 @@
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1282,24 +1289,27 @@
       <c r="E2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
         <v>9</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>2020</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>9</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>2020</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1315,26 +1325,29 @@
       <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
         <v>12</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>2020</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>10</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>2020</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1350,26 +1363,29 @@
       <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
       <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
         <v>2021</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>2021</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1385,24 +1401,27 @@
       <c r="E5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
         <v>4</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>2021</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>2021</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1418,26 +1437,29 @@
       <c r="E6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
         <v>6</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>2021</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>2021</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1453,24 +1475,27 @@
       <c r="E7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
         <v>8</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>2021</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>6</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>2021</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -1484,26 +1509,29 @@
       <c r="E8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
         <v>9</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>2021</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>8</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>2021</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -1517,23 +1545,26 @@
       <c r="E9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>4</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>2021</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18"/>
+    <row r="18" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>